<commit_message>
login page perfect_ with Phases
</commit_message>
<xml_diff>
--- a/backend/data/logs.xlsx
+++ b/backend/data/logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -658,9 +658,841 @@
         <v>None</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B9" t="str">
+        <v>01:24:20</v>
+      </c>
+      <c r="C9" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D9" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="F9" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G9" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H9" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I9" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J9" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B10" t="str">
+        <v>01:24:21</v>
+      </c>
+      <c r="C10" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D10" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="E10" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F10" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G10" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H10" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I10" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J10" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B11" t="str">
+        <v>01:24:21</v>
+      </c>
+      <c r="C11" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D11" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F11" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G11" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H11" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I11" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J11" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B12" t="str">
+        <v>01:24:22</v>
+      </c>
+      <c r="C12" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="D12" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="E12" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="F12" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G12" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H12" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I12" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J12" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B13" t="str">
+        <v>01:24:22</v>
+      </c>
+      <c r="C13" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="D13" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E13" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="F13" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G13" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H13" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I13" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J13" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B14" t="str">
+        <v>01:24:23</v>
+      </c>
+      <c r="C14" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="D14" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="F14" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G14" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H14" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I14" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J14" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B15" t="str">
+        <v>01:24:23</v>
+      </c>
+      <c r="C15" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="D15" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="E15" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="F15" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G15" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H15" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I15" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J15" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B16" t="str">
+        <v>01:24:24</v>
+      </c>
+      <c r="C16" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D16" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="E16" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="F16" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G16" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H16" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I16" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J16" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B17" t="str">
+        <v>01:24:24</v>
+      </c>
+      <c r="C17" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="D17" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="E17" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="F17" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G17" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H17" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I17" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J17" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B18" t="str">
+        <v>01:24:25</v>
+      </c>
+      <c r="C18" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="D18" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="E18" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="F18" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G18" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H18" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I18" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J18" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B19" t="str">
+        <v>01:56:54</v>
+      </c>
+      <c r="C19" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D19" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="E19" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F19" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G19" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H19" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I19" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J19" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B20" t="str">
+        <v>01:56:55</v>
+      </c>
+      <c r="C20" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="D20" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E20" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="F20" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G20" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H20" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I20" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J20" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B21" t="str">
+        <v>01:56:55</v>
+      </c>
+      <c r="C21" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D21" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E21" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F21" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G21" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H21" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I21" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J21" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B22" t="str">
+        <v>01:56:56</v>
+      </c>
+      <c r="C22" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="D22" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E22" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F22" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G22" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H22" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I22" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J22" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B23" t="str">
+        <v>01:56:56</v>
+      </c>
+      <c r="C23" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="D23" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="E23" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="F23" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G23" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H23" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I23" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J23" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B24" t="str">
+        <v>01:56:56</v>
+      </c>
+      <c r="C24" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D24" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E24" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="F24" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G24" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H24" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I24" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J24" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B25" t="str">
+        <v>01:56:57</v>
+      </c>
+      <c r="C25" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="D25" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="E25" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="F25" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G25" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H25" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I25" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J25" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B26" t="str">
+        <v>01:56:57</v>
+      </c>
+      <c r="C26" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D26" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="E26" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="F26" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G26" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H26" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I26" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J26" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B27" t="str">
+        <v>01:56:58</v>
+      </c>
+      <c r="C27" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D27" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="E27" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="F27" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G27" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H27" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I27" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J27" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B28" t="str">
+        <v>01:56:58</v>
+      </c>
+      <c r="C28" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D28" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E28" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F28" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G28" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H28" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I28" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J28" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B29" t="str">
+        <v>01:56:58</v>
+      </c>
+      <c r="C29" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D29" t="str">
+        <v>227.00</v>
+      </c>
+      <c r="E29" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F29" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G29" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H29" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I29" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J29" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B30" t="str">
+        <v>01:56:59</v>
+      </c>
+      <c r="C30" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D30" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="E30" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F30" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G30" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H30" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I30" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J30" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B31" t="str">
+        <v>01:56:59</v>
+      </c>
+      <c r="C31" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D31" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="E31" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="F31" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G31" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H31" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I31" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J31" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B32" t="str">
+        <v>01:57:00</v>
+      </c>
+      <c r="C32" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="D32" t="str">
+        <v>231.00</v>
+      </c>
+      <c r="E32" t="str">
+        <v>233.00</v>
+      </c>
+      <c r="F32" t="str">
+        <v>14.200</v>
+      </c>
+      <c r="G32" t="str">
+        <v>13.800</v>
+      </c>
+      <c r="H32" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I32" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J32" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="B33" t="str">
+        <v>01:57:00</v>
+      </c>
+      <c r="C33" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="D33" t="str">
+        <v>230.00</v>
+      </c>
+      <c r="E33" t="str">
+        <v>232.00</v>
+      </c>
+      <c r="F33" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G33" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H33" t="str">
+        <v>15.100</v>
+      </c>
+      <c r="I33" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J33" t="str">
+        <v>None</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="B34" t="str">
+        <v>07:30:00</v>
+      </c>
+      <c r="C34" t="str">
+        <v>230.50</v>
+      </c>
+      <c r="D34" t="str">
+        <v>228.30</v>
+      </c>
+      <c r="E34" t="str">
+        <v>232.10</v>
+      </c>
+      <c r="F34" t="str">
+        <v>15.200</v>
+      </c>
+      <c r="G34" t="str">
+        <v>14.800</v>
+      </c>
+      <c r="H34" t="str">
+        <v>16.100</v>
+      </c>
+      <c r="I34" t="str">
+        <v>NO</v>
+      </c>
+      <c r="J34" t="str">
+        <v>None</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>